<commit_message>
Updated Parts List --Arthur
git-svn-id: http://cd-net.net/CPE496/trunk@126 05b6d0e0-c345-4a8e-a5b7-579c8bd0b646
</commit_message>
<xml_diff>
--- a/Parts List (Keep Me Updated).xlsx
+++ b/Parts List (Keep Me Updated).xlsx
@@ -18,9 +18,11 @@
     <definedName name="gr10_1.values_3" localSheetId="0">Sheet1!$A$1:$D$21</definedName>
     <definedName name="gr10_1.values_4" localSheetId="0">Sheet1!$A$1:$D$21</definedName>
     <definedName name="gr10_1.values_5" localSheetId="0">Sheet1!$A$1:$D$21</definedName>
-    <definedName name="partslist" localSheetId="0">Sheet1!$A$1:$D$33</definedName>
+    <definedName name="partslist" localSheetId="0">Sheet1!$A$1:$D$37</definedName>
     <definedName name="partslist" localSheetId="1">Sheet2!$A$1:$D$29</definedName>
     <definedName name="partslist_1" localSheetId="0">Sheet1!$A$1:$D$29</definedName>
+    <definedName name="partslist_2" localSheetId="0">Sheet1!$A$1:$D$29</definedName>
+    <definedName name="partslist_3" localSheetId="0">Sheet1!$A$1:$D$29</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="143">
   <si>
     <t>Value</t>
   </si>
@@ -46,9 +48,6 @@
     <t>Device</t>
   </si>
   <si>
-    <t>3,81/1,4</t>
-  </si>
-  <si>
     <t>MB4S</t>
   </si>
   <si>
@@ -64,13 +63,10 @@
     <t>R12</t>
   </si>
   <si>
-    <t>U$1</t>
-  </si>
-  <si>
     <t>MICROSD</t>
   </si>
   <si>
-    <t>U$2</t>
+    <t>ATMEGA328</t>
   </si>
   <si>
     <t>REG3.3V</t>
@@ -163,9 +159,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>See transformers.txt</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
@@ -175,9 +168,6 @@
     <t>http://search.digikey.com/us/en/products/961206-6404-AR/3M9459-ND/2071500</t>
   </si>
   <si>
-    <t>Other Notes</t>
-  </si>
-  <si>
     <t>Order at least 10</t>
   </si>
   <si>
@@ -193,15 +183,9 @@
     <t>Price Per Board</t>
   </si>
   <si>
-    <t>Actual Total</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>Leaving unpopulated for now</t>
-  </si>
-  <si>
     <t>ISP header</t>
   </si>
   <si>
@@ -256,9 +240,6 @@
     <t>Case</t>
   </si>
   <si>
-    <t>Plugs</t>
-  </si>
-  <si>
     <t>Wire</t>
   </si>
   <si>
@@ -313,9 +294,15 @@
     <t>radio</t>
   </si>
   <si>
+    <t>AT86RF231</t>
+  </si>
+  <si>
     <t>http://parts.digikey.com/1/parts/1790682-balun-ember351-357-0805-smd-748421245.html</t>
   </si>
   <si>
+    <t>BALUN</t>
+  </si>
+  <si>
     <t>balun</t>
   </si>
   <si>
@@ -388,15 +375,9 @@
     <t>ANTENNA2SMD</t>
   </si>
   <si>
-    <t>U$5</t>
-  </si>
-  <si>
     <t>AT86RF231(RADIO)AT86RF231</t>
   </si>
   <si>
-    <t>U$3</t>
-  </si>
-  <si>
     <t>ATMEGA32832A</t>
   </si>
   <si>
@@ -421,9 +402,6 @@
     <t>WE-BAL</t>
   </si>
   <si>
-    <t>U$4</t>
-  </si>
-  <si>
     <t>C3, C4, C10, C11</t>
   </si>
   <si>
@@ -434,17 +412,76 @@
   </si>
   <si>
     <t>RF-TX, STATUS</t>
+  </si>
+  <si>
+    <t>For 3 Boards</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Cost overhead from spare/unused parts</t>
+  </si>
+  <si>
+    <t>ANTENNA</t>
+  </si>
+  <si>
+    <t>115V -&gt; 5V</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/us/en/products/UX60A-MB-5ST/H2961CT-ND/597540</t>
+  </si>
+  <si>
+    <t>mini USB</t>
+  </si>
+  <si>
+    <t>Minimum Order</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/us/en/products/GRM188R71H103KA01D/490-1512-1-ND/587862</t>
+  </si>
+  <si>
+    <t>10nF Cap</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/us/en/products/Q-712/Q527-ND/2180784</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/us/en/products/703W-00%2F07/Q335-ND/1164206</t>
+  </si>
+  <si>
+    <t>To Outlet</t>
+  </si>
+  <si>
+    <t>Euro IN</t>
+  </si>
+  <si>
+    <t>Edison Out</t>
+  </si>
+  <si>
+    <t>To Device</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/us/en/products/CU-1874-B/377-1165-ND/387084</t>
+  </si>
+  <si>
+    <t>Enclosure</t>
+  </si>
+  <si>
+    <t>PTH3MM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,6 +522,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -511,25 +554,39 @@
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -542,39 +599,47 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="partslist_3" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values_4" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="partslist" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="partslist_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="partslist_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="partslist" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values_3" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values_5" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values_4" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="partslist" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -864,29 +929,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="75.5703125" style="4" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="4.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="75.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -895,55 +960,66 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>45</v>
+      <c r="F1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="7">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="F2" s="7">
+        <f>E2*A3</f>
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="G2" s="7">
+        <f>F2*3</f>
+        <v>13.559999999999999</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2">
+        <f>3*A3</f>
         <v>3</v>
-      </c>
-      <c r="B2"/>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -951,33 +1027,36 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="2">
-        <v>4.5199999999999996</v>
-      </c>
-      <c r="F3" s="2">
-        <f>E3*A3</f>
-        <v>4.5199999999999996</v>
-      </c>
-      <c r="G3" s="2">
+        <v>127</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="F3" s="7">
+        <f>E3*A4</f>
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="G3" s="7">
         <f>F3*3</f>
-        <v>13.559999999999999</v>
+        <v>2.532</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>39</v>
+        <v>88</v>
+      </c>
+      <c r="I3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -985,36 +1064,37 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.84399999999999997</v>
-      </c>
-      <c r="F4" s="2">
-        <f>E4*A27</f>
-        <v>2.532</v>
-      </c>
-      <c r="G4" s="2">
+        <v>84</v>
+      </c>
+      <c r="E4" s="9">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="F4" s="7">
+        <f>E4*A5</f>
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="G4" s="7">
         <f>F4*3</f>
-        <v>7.5960000000000001</v>
+        <v>14.190000000000001</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I4" t="s">
-        <v>94</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>46</v>
+        <v>83</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4">
+        <f>3*A5</f>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1022,33 +1102,37 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="8">
-        <v>4.7300000000000004</v>
-      </c>
-      <c r="F5" s="2">
-        <f>E5*A5</f>
-        <v>4.7300000000000004</v>
-      </c>
-      <c r="G5" s="2">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7">
+        <v>3.83</v>
+      </c>
+      <c r="F5" s="7">
+        <f>E5*A6</f>
+        <v>3.83</v>
+      </c>
+      <c r="G5" s="7">
         <f>F5*3</f>
-        <v>14.190000000000001</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I5" t="s">
-        <v>90</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>40</v>
+        <v>11.49</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5">
+        <f>3*A6</f>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1056,427 +1140,465 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2">
-        <v>3.83</v>
-      </c>
-      <c r="F6" s="2">
-        <f>E6*A4</f>
-        <v>3.83</v>
-      </c>
-      <c r="G6" s="2">
+        <v>49</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.39</v>
+      </c>
+      <c r="F6" s="7">
+        <f>E6*A7</f>
+        <v>0.78</v>
+      </c>
+      <c r="G6" s="7">
         <f>F6*3</f>
-        <v>11.49</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>39</v>
+        <v>2.34</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.39</v>
-      </c>
-      <c r="F7" s="2">
-        <f>E7*A5</f>
-        <v>0.39</v>
-      </c>
-      <c r="G7" s="2">
-        <f>F7*3</f>
-        <v>1.17</v>
+        <v>79</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="F7" s="7">
+        <f>E7*A8</f>
+        <v>0.05</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1.25</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>75</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75">
       <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="8">
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="F8" s="7">
+        <f>E8*A9</f>
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="G8" s="8">
+        <v>3.06</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="F9" s="7">
+        <f>E9*A10</f>
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1.53</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F10" s="7">
+        <f>E10*A11</f>
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75">
+      <c r="A11">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="8">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="F11" s="7">
+        <f>E11*A12</f>
+        <v>0.09</v>
+      </c>
+      <c r="G11" s="8">
+        <v>2.25</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="F8" s="2">
-        <f>E8*A7</f>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1.25</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" t="s">
-        <v>106</v>
-      </c>
-      <c r="E9" s="10">
-        <v>3.0599999999999999E-2</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="10">
-        <v>3.06</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1.5299999999999999E-2</v>
-      </c>
-      <c r="F10" s="2">
-        <f>E10*A8</f>
-        <v>3.0599999999999999E-2</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1.53</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B12" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>109</v>
-      </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
-      </c>
-      <c r="E12" s="10">
+        <v>120</v>
+      </c>
+      <c r="E12" s="7">
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="10">
+      <c r="F12" s="7">
+        <f>E12*A13</f>
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="G12" s="7">
         <v>2.25</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>40</v>
+      <c r="H12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" t="s">
+        <v>38</v>
       </c>
       <c r="K12" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>113</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B13"/>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>128</v>
-      </c>
-      <c r="E13" s="2">
-        <v>2.2499999999999999E-2</v>
-      </c>
-      <c r="F13" s="2">
-        <f>E13*A9</f>
-        <v>0.09</v>
-      </c>
-      <c r="G13" s="2">
-        <v>2.25</v>
-      </c>
-      <c r="H13" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="J13" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" t="s">
-        <v>79</v>
+      <c r="E13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14"/>
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>53</v>
+        <v>69</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F14" s="7">
+        <f>E14*A15</f>
+        <v>1.8</v>
+      </c>
+      <c r="G14" s="7">
+        <f>3*F14</f>
+        <v>5.4</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14">
+        <f>3*A15</f>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="F15" s="2">
-        <f>E15*A10</f>
-        <v>0.9</v>
-      </c>
-      <c r="G15" s="2">
-        <f>3*F15</f>
-        <v>2.7</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I15" t="s">
-        <v>74</v>
-      </c>
-      <c r="J15" t="s">
-        <v>40</v>
+        <v>121</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="F15" s="7">
+        <f>E15*A16</f>
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="G15" s="7">
+        <v>3.58</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="D16" t="s">
-        <v>129</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="F16" s="2">
-        <f>E16*A11</f>
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="G16" s="2">
-        <v>3.58</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
+      </c>
+      <c r="E16" s="10">
+        <v>4.28</v>
+      </c>
+      <c r="F16" s="7">
+        <f>E16*A17</f>
+        <v>4.28</v>
+      </c>
+      <c r="G16" s="7">
+        <f>F16*3</f>
+        <v>12.84</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16">
+        <f>3*A17</f>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17">
         <v>1</v>
       </c>
-      <c r="B17"/>
+      <c r="B17" t="s">
+        <v>113</v>
+      </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
-      </c>
-      <c r="E17" s="6">
-        <v>4.28</v>
-      </c>
-      <c r="F17" s="2">
-        <f>E17*A12</f>
-        <v>8.56</v>
-      </c>
-      <c r="G17" s="3">
-        <f>F17*3</f>
-        <v>25.68</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>41</v>
+        <v>114</v>
+      </c>
+      <c r="E17" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="F17" s="7">
+        <f>E17*A18</f>
+        <v>9</v>
+      </c>
+      <c r="G17" s="7">
+        <f>3*F17</f>
+        <v>27</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17">
+        <f>3*A18</f>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>121</v>
-      </c>
-      <c r="E18" s="11">
-        <v>4.5</v>
-      </c>
-      <c r="F18" s="11">
-        <f>E18*A40</f>
-        <v>4.5</v>
-      </c>
-      <c r="G18" s="2">
-        <f>3*F18</f>
-        <v>13.5</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I18" t="s">
-        <v>102</v>
-      </c>
-      <c r="J18" t="s">
-        <v>40</v>
+        <v>122</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="F18" s="7">
+        <f>E18*A19</f>
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="G18" s="7">
+        <v>1.17</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1484,153 +1606,172 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>130</v>
-      </c>
-      <c r="E19" s="6">
+        <v>123</v>
+      </c>
+      <c r="E19" s="7">
         <v>0.11700000000000001</v>
       </c>
-      <c r="F19" s="2">
-        <f>E19*A13</f>
-        <v>0.46800000000000003</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="F19" s="7">
+        <f>E19*A20</f>
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="G19" s="7">
         <v>1.17</v>
       </c>
-      <c r="H19" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="H19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75">
       <c r="A20">
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="F20" s="2">
-        <f>E20*A14</f>
-        <v>0.35100000000000003</v>
-      </c>
-      <c r="G20" s="2">
-        <v>1.17</v>
+        <v>40</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="F20" s="7">
+        <f>E20*A21</f>
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="G20" s="7">
+        <v>4.1399999999999997</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1.94</v>
+      </c>
+      <c r="F21" s="7">
+        <f>E21*A22</f>
+        <v>1.94</v>
+      </c>
+      <c r="G21" s="7">
+        <f>F21*3</f>
+        <v>5.82</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21">
+        <f>3*A22</f>
         <v>3</v>
       </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="F21" s="2">
-        <f>E21*A16</f>
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="G21" s="2">
-        <f>F21*3</f>
-        <v>3.42</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+    </row>
+    <row r="22" spans="1:11" ht="15.75">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1.94</v>
-      </c>
-      <c r="F22" s="2">
-        <f>E22*A17</f>
-        <v>1.94</v>
-      </c>
-      <c r="G22" s="2">
-        <f>F22*3</f>
-        <v>5.82</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>39</v>
+        <v>116</v>
+      </c>
+      <c r="E22" s="12">
+        <v>1.0229999999999999</v>
+      </c>
+      <c r="F22" s="7">
+        <f>E22*A23</f>
+        <v>3.069</v>
+      </c>
+      <c r="G22" s="12">
+        <v>10.23</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>122</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B23"/>
       <c r="C23" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
+        <v>98</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1638,33 +1779,37 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="2">
+        <v>20</v>
+      </c>
+      <c r="E24" s="7">
         <v>0.66</v>
       </c>
-      <c r="F24" s="2">
-        <f>E24*A18</f>
+      <c r="F24" s="7">
+        <f t="shared" ref="F24:F27" si="0">E24*A24</f>
         <v>0.66</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="7">
         <f>F24*3</f>
         <v>1.98</v>
       </c>
-      <c r="H24" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I24" s="4" t="s">
+      <c r="H24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J24" s="4" t="s">
-        <v>39</v>
+      <c r="I24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24">
+        <f>3*A24</f>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1672,35 +1817,35 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" t="s">
         <v>63</v>
       </c>
-      <c r="D25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="2">
+      <c r="E25" s="7">
         <v>1.5800000000000002E-2</v>
       </c>
-      <c r="F25" s="2">
-        <f>E25*A19</f>
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="G25" s="2">
+      <c r="F25" s="7">
+        <f t="shared" si="0"/>
+        <v>7.9000000000000015E-2</v>
+      </c>
+      <c r="G25" s="7">
         <v>1.58</v>
       </c>
-      <c r="H25" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>79</v>
+      <c r="H25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1708,35 +1853,35 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="2">
+        <v>6</v>
+      </c>
+      <c r="E26" s="7">
         <v>1.5800000000000002E-2</v>
       </c>
-      <c r="F26" s="2">
-        <f>E26*A20</f>
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="G26" s="2">
+      <c r="F26" s="7">
+        <f t="shared" si="0"/>
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="G26" s="7">
         <v>1.58</v>
       </c>
-      <c r="H26" s="4" t="s">
-        <v>68</v>
+      <c r="H26" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="I26" t="s">
-        <v>67</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>79</v>
+        <v>61</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1747,32 +1892,32 @@
         <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D27" t="s">
-        <v>114</v>
-      </c>
-      <c r="E27" s="2">
+        <v>109</v>
+      </c>
+      <c r="E27" s="7">
         <v>1.5800000000000002E-2</v>
       </c>
-      <c r="F27" s="2">
-        <f>E27*A21</f>
-        <v>3.1600000000000003E-2</v>
-      </c>
-      <c r="G27" s="2">
+      <c r="F27" s="7">
+        <f t="shared" si="0"/>
+        <v>4.7400000000000005E-2</v>
+      </c>
+      <c r="G27" s="7">
         <v>1.58</v>
       </c>
-      <c r="H27" s="4" t="s">
-        <v>66</v>
+      <c r="H27" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="I27" t="s">
-        <v>95</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>79</v>
+        <v>90</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1780,13 +1925,28 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D28" t="s">
-        <v>125</v>
+        <v>118</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1794,33 +1954,37 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C29" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D29" t="s">
-        <v>127</v>
-      </c>
-      <c r="E29" s="2">
+        <v>86</v>
+      </c>
+      <c r="E29" s="7">
         <v>2.58</v>
       </c>
-      <c r="F29" s="2">
-        <f>E29*A26</f>
+      <c r="F29" s="7">
+        <f>E29*A29</f>
         <v>2.58</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="7">
         <f>F29*3</f>
         <v>7.74</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="I29" t="s">
-        <v>92</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>40</v>
+        <v>87</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K29">
+        <f>3*A29</f>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1829,42 +1993,133 @@
       <c r="C30"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:11">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
+    <row r="31" spans="1:11" ht="15.75">
+      <c r="A31" s="3">
+        <v>1</v>
+      </c>
       <c r="D31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
+        <v>136</v>
+      </c>
+      <c r="E31" s="12">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="F31" s="7">
+        <f>E31*A31</f>
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="G31" s="12">
+        <v>7.97</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I31" t="s">
+        <v>137</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15.75">
+      <c r="A32" s="3">
+        <v>1</v>
+      </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>139</v>
+      </c>
+      <c r="E32" s="12">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="F32" s="7">
+        <f>E32*A32</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="G32" s="7">
+        <f>F32*3</f>
+        <v>3.3899999999999997</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I32" t="s">
+        <v>138</v>
+      </c>
+      <c r="K32">
+        <f>3*A32</f>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
-      <c r="D33" s="4" t="s">
-        <v>71</v>
+      <c r="D33" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:11">
-      <c r="D34" s="7" t="s">
-        <v>19</v>
+      <c r="A34" s="3">
+        <v>1</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="7">
+        <v>3</v>
+      </c>
+      <c r="F34" s="7">
+        <f>E34*A34</f>
+        <v>3</v>
+      </c>
+      <c r="G34" s="7">
+        <f>F34*3</f>
+        <v>9</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="K34">
+        <f>3*A34</f>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:11">
-      <c r="K35"/>
+      <c r="D35" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="F36" s="7">
+        <f>SUM(F2:F33)</f>
+        <v>41.62360000000001</v>
+      </c>
+      <c r="G36" s="7">
+        <f>SUM(G2:G33)</f>
+        <v>153.02200000000005</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="G37" s="11">
+        <f>F36*3-G36</f>
+        <v>-28.151200000000017</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="4">
-        <v>1</v>
-      </c>
       <c r="B40" s="1"/>
     </row>
   </sheetData>
@@ -1872,25 +2127,30 @@
     <sortCondition ref="C1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="H17" r:id="rId1"/>
-    <hyperlink ref="H16" r:id="rId2"/>
+    <hyperlink ref="H16" r:id="rId1"/>
+    <hyperlink ref="H15" r:id="rId2"/>
     <hyperlink ref="H24" r:id="rId3"/>
-    <hyperlink ref="H6" r:id="rId4"/>
-    <hyperlink ref="H3" r:id="rId5"/>
-    <hyperlink ref="H22" r:id="rId6"/>
-    <hyperlink ref="H21" r:id="rId7"/>
-    <hyperlink ref="H7" r:id="rId8"/>
-    <hyperlink ref="H15" r:id="rId9"/>
-    <hyperlink ref="H5" r:id="rId10"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H2" r:id="rId5"/>
+    <hyperlink ref="H21" r:id="rId6"/>
+    <hyperlink ref="H20" r:id="rId7"/>
+    <hyperlink ref="H6" r:id="rId8"/>
+    <hyperlink ref="H14" r:id="rId9"/>
+    <hyperlink ref="H4" r:id="rId10"/>
     <hyperlink ref="H29" r:id="rId11"/>
-    <hyperlink ref="H4" r:id="rId12"/>
-    <hyperlink ref="H8" r:id="rId13"/>
-    <hyperlink ref="H12" r:id="rId14"/>
-    <hyperlink ref="H9" r:id="rId15"/>
-    <hyperlink ref="H18" r:id="rId16"/>
+    <hyperlink ref="H3" r:id="rId12"/>
+    <hyperlink ref="H7" r:id="rId13"/>
+    <hyperlink ref="H11" r:id="rId14"/>
+    <hyperlink ref="H8" r:id="rId15"/>
+    <hyperlink ref="H17" r:id="rId16"/>
+    <hyperlink ref="H22" r:id="rId17"/>
+    <hyperlink ref="H10" r:id="rId18"/>
+    <hyperlink ref="H32" r:id="rId19"/>
+    <hyperlink ref="H31" r:id="rId20"/>
+    <hyperlink ref="H34" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -1898,7 +2158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection sqref="A1:D29"/>
     </sheetView>
   </sheetViews>
@@ -1914,7 +2174,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1923,18 +2183,21 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1942,13 +2205,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1956,13 +2219,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1970,13 +2233,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1984,55 +2247,55 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" t="s">
         <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2040,119 +2303,122 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>113</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="D16" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
         <v>1</v>
       </c>
+      <c r="B17" t="s">
+        <v>113</v>
+      </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2160,13 +2426,13 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2174,27 +2440,27 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2202,27 +2468,24 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>122</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2230,13 +2493,13 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2244,13 +2507,13 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" t="s">
         <v>63</v>
-      </c>
-      <c r="D25" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2258,13 +2521,13 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2275,10 +2538,10 @@
         <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D27" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2286,13 +2549,13 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D28" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2300,13 +2563,13 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C29" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D29" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2338,16 +2601,16 @@
         <v>1.9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Parts List in Trunk to represent what we really ordered for Rev A.
--Arthur

git-svn-id: http://cd-net.net/CPE496/trunk@139 05b6d0e0-c345-4a8e-a5b7-579c8bd0b646
</commit_message>
<xml_diff>
--- a/Parts List (Keep Me Updated).xlsx
+++ b/Parts List (Keep Me Updated).xlsx
@@ -18,7 +18,7 @@
     <definedName name="gr10_1.values_3" localSheetId="0">Sheet1!$A$1:$D$21</definedName>
     <definedName name="gr10_1.values_4" localSheetId="0">Sheet1!$A$1:$D$21</definedName>
     <definedName name="gr10_1.values_5" localSheetId="0">Sheet1!$A$1:$D$21</definedName>
-    <definedName name="partslist" localSheetId="0">Sheet1!$A$1:$D$37</definedName>
+    <definedName name="partslist" localSheetId="0">Sheet1!$A$1:$D$39</definedName>
     <definedName name="partslist" localSheetId="1">Sheet2!$A$1:$D$29</definedName>
     <definedName name="partslist_1" localSheetId="0">Sheet1!$A$1:$D$29</definedName>
     <definedName name="partslist_2" localSheetId="0">Sheet1!$A$1:$D$29</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="157">
   <si>
     <t>Value</t>
   </si>
@@ -144,18 +144,12 @@
     <t>transformer</t>
   </si>
   <si>
-    <t>http://parts.digikey.com/1/parts/1422327-ic-rect-bridge-0-5a-400v-4soic-mb4s.html</t>
-  </si>
-  <si>
     <t>bridge rectifier</t>
   </si>
   <si>
     <t>Already have</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -330,9 +324,6 @@
     <t>1 uF Caps</t>
   </si>
   <si>
-    <t>http://parts.digikey.com/1/parts/1501976-ic-usb-fs-serial-uart-28-ssop-ft232rl-reel.html</t>
-  </si>
-  <si>
     <t>USB-Serial Chip</t>
   </si>
   <si>
@@ -444,9 +435,6 @@
     <t>10nF Cap</t>
   </si>
   <si>
-    <t>http://search.digikey.com/us/en/products/Q-712/Q527-ND/2180784</t>
-  </si>
-  <si>
     <t>http://search.digikey.com/us/en/products/703W-00%2F07/Q335-ND/1164206</t>
   </si>
   <si>
@@ -462,9 +450,6 @@
     <t>To Device</t>
   </si>
   <si>
-    <t>http://search.digikey.com/us/en/products/CU-1874-B/377-1165-ND/387084</t>
-  </si>
-  <si>
     <t>Enclosure</t>
   </si>
   <si>
@@ -475,17 +460,66 @@
   </si>
   <si>
     <t>See Provided Rubric</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/us/en/products/RNCP0603FTD7K50/RNCP0603FTD7K50CT-ND/2240474</t>
+  </si>
+  <si>
+    <t>Alternate Resistor</t>
+  </si>
+  <si>
+    <t>7.5K Alternate</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/us/en/products/RNCP0603FTD14K0/RNCP0603FTD14K0CT-ND/2240484</t>
+  </si>
+  <si>
+    <t>14K Alternate</t>
+  </si>
+  <si>
+    <t>Order at least 25</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/us/en/products/4300.0701/486-1082-ND/1207600</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/us/en/products/03540901ZXGY/F3131-ND/554005</t>
+  </si>
+  <si>
+    <t>fuse holder</t>
+  </si>
+  <si>
+    <t>Fuse Holder</t>
+  </si>
+  <si>
+    <t>Order at least 5</t>
+  </si>
+  <si>
+    <t>Fuse</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/us/en/products/3SB%2015-R/507-1537-ND/1009761</t>
+  </si>
+  <si>
+    <t>15A Fuse</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/us/en/products/133,BK/SR133B-ND/95399</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=112820000&amp;uq=634689795876532809</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=112820148&amp;uq=634689795876532809</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -572,28 +606,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -608,7 +640,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="partslist_3" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -620,35 +652,35 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="partslist_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="partslist_3" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values_3" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="partslist_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="partslist" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values_3" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values_5" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="gr10-1.values_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -936,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35:G35"/>
+    <sheetView tabSelected="1" topLeftCell="F30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -948,12 +980,12 @@
     <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="3" customWidth="1"/>
     <col min="4" max="4" width="27" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="11" customWidth="1"/>
     <col min="8" max="8" width="75.5703125" style="3" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="3" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="31.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
@@ -971,14 +1003,14 @@
       <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>124</v>
+      <c r="F1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>121</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>15</v>
@@ -987,10 +1019,10 @@
         <v>31</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1006,14 +1038,14 @@
       <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="11">
         <v>4.5199999999999996</v>
       </c>
-      <c r="F2" s="7">
-        <f>E2*A3</f>
+      <c r="F2" s="11">
+        <f>E2*A2</f>
         <v>4.5199999999999996</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="11">
         <f>F2*3</f>
         <v>13.559999999999999</v>
       </c>
@@ -1023,11 +1055,8 @@
       <c r="I2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="K2">
-        <f>3*A3</f>
+        <f>3*A2</f>
         <v>3</v>
       </c>
     </row>
@@ -1036,36 +1065,32 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E3" s="7">
+        <v>124</v>
+      </c>
+      <c r="E3" s="11">
         <v>0.84399999999999997</v>
       </c>
-      <c r="F3" s="7">
-        <f>E3*A4</f>
+      <c r="F3" s="11">
+        <f t="shared" ref="F3:F12" si="0">E3*A3</f>
         <v>0.84399999999999997</v>
       </c>
-      <c r="G3" s="7">
-        <f>F3*3</f>
-        <v>2.532</v>
+      <c r="G3" s="11">
+        <v>8.44</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1073,77 +1098,71 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="9">
+        <v>82</v>
+      </c>
+      <c r="E4" s="7">
         <v>4.7300000000000004</v>
       </c>
-      <c r="F4" s="7">
-        <f>E4*A5</f>
+      <c r="F4" s="11">
+        <f t="shared" si="0"/>
         <v>4.7300000000000004</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="11">
         <f>F4*3</f>
         <v>14.190000000000001</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="K4">
+        <f>3*A4</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="11">
+        <v>3.83</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="0"/>
+        <v>3.83</v>
+      </c>
+      <c r="G5" s="11">
+        <f>F5*3</f>
+        <v>11.49</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5">
         <f>3*A5</f>
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="7">
-        <v>3.83</v>
-      </c>
-      <c r="F5" s="7">
-        <f>E5*A6</f>
-        <v>3.83</v>
-      </c>
-      <c r="G5" s="7">
-        <f>F5*3</f>
-        <v>11.49</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K5">
-        <f>3*A6</f>
-        <v>3</v>
-      </c>
-    </row>
     <row r="6" spans="1:11">
       <c r="A6">
         <v>1</v>
@@ -1155,30 +1174,26 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="7">
+        <v>47</v>
+      </c>
+      <c r="E6" s="11">
         <v>0.39</v>
       </c>
-      <c r="F6" s="7">
-        <f>E6*A7</f>
-        <v>0.78</v>
-      </c>
-      <c r="G6" s="7">
-        <f>F6*3</f>
-        <v>2.34</v>
+      <c r="F6" s="11">
+        <f t="shared" si="0"/>
+        <v>0.39</v>
+      </c>
+      <c r="G6" s="11">
+        <v>3.15</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1189,32 +1204,29 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
         <v>77</v>
       </c>
-      <c r="D7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="F7" s="7">
-        <f>E7*A8</f>
-        <v>0.05</v>
-      </c>
-      <c r="G7" s="7">
-        <v>1.25</v>
+      <c r="E7" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="0"/>
+        <v>1.52E-2</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0.76</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75">
@@ -1222,35 +1234,32 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="0"/>
+        <v>7.4800000000000005E-2</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1.87</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E8" s="8">
-        <v>3.0599999999999999E-2</v>
-      </c>
-      <c r="F8" s="7">
-        <f>E8*A9</f>
-        <v>3.0599999999999999E-2</v>
-      </c>
-      <c r="G8" s="8">
-        <v>3.06</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="K8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1261,32 +1270,29 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="11">
         <v>1.5299999999999999E-2</v>
       </c>
-      <c r="F9" s="7">
-        <f>E9*A10</f>
+      <c r="F9" s="11">
+        <f t="shared" si="0"/>
         <v>1.5299999999999999E-2</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="11">
         <v>1.53</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>73</v>
+      <c r="H9" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75">
@@ -1294,35 +1300,32 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="12">
+        <v>100</v>
+      </c>
+      <c r="E10" s="8">
         <v>1.4E-2</v>
       </c>
-      <c r="F10" s="7">
-        <f>E10*A11</f>
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="G10" s="7">
+      <c r="F10" s="11">
+        <f t="shared" si="0"/>
+        <v>1.4E-2</v>
+      </c>
+      <c r="G10" s="11">
         <v>1.4</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="K10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75">
@@ -1330,35 +1333,32 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E11" s="8">
-        <v>2.2499999999999999E-2</v>
-      </c>
-      <c r="F11" s="7">
-        <f>E11*A12</f>
-        <v>0.09</v>
+        <v>1.38E-2</v>
+      </c>
+      <c r="F11" s="11">
+        <f t="shared" si="0"/>
+        <v>2.76E-2</v>
       </c>
       <c r="G11" s="8">
-        <v>2.25</v>
+        <v>1.38</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="I11" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="K11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1366,35 +1366,33 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>120</v>
-      </c>
-      <c r="E12" s="7">
-        <v>2.2499999999999999E-2</v>
-      </c>
-      <c r="F12" s="7">
-        <f>E12*A13</f>
-        <v>6.7500000000000004E-2</v>
-      </c>
-      <c r="G12" s="7">
-        <v>2.25</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>71</v>
+        <v>117</v>
+      </c>
+      <c r="E12" s="11">
+        <v>1.38E-2</v>
+      </c>
+      <c r="F12" s="11">
+        <f t="shared" si="0"/>
+        <v>5.5199999999999999E-2</v>
+      </c>
+      <c r="G12" s="11">
+        <v>1.38</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="I12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12"/>
+      <c r="K12" t="s">
         <v>70</v>
-      </c>
-      <c r="J12" t="s">
-        <v>38</v>
-      </c>
-      <c r="K12" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1403,22 +1401,22 @@
       </c>
       <c r="B13"/>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>47</v>
+        <v>76</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>32</v>
@@ -1429,37 +1427,35 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="7">
+        <v>67</v>
+      </c>
+      <c r="E14" s="11">
         <v>0.9</v>
       </c>
-      <c r="F14" s="7">
-        <f>E14*A15</f>
-        <v>1.8</v>
-      </c>
-      <c r="G14" s="7">
+      <c r="F14" s="11">
+        <f t="shared" ref="F14:F22" si="1">E14*A14</f>
+        <v>0.9</v>
+      </c>
+      <c r="G14" s="11">
         <f>3*F14</f>
-        <v>5.4</v>
+        <v>2.7</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I14" t="s">
-        <v>67</v>
-      </c>
-      <c r="J14" t="s">
-        <v>38</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="J14"/>
       <c r="K14">
-        <f>3*A15</f>
-        <v>6</v>
+        <f>3*A14</f>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1467,22 +1463,22 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D15" t="s">
-        <v>121</v>
-      </c>
-      <c r="E15" s="7">
+        <v>118</v>
+      </c>
+      <c r="E15" s="11">
         <v>0.35799999999999998</v>
       </c>
-      <c r="F15" s="7">
-        <f>E15*A16</f>
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="G15" s="7">
+      <c r="F15" s="11">
+        <f t="shared" si="1"/>
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="G15" s="11">
         <v>3.58</v>
       </c>
       <c r="H15" s="4" t="s">
@@ -1491,11 +1487,8 @@
       <c r="I15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="K15" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1503,24 +1496,24 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" s="10">
-        <v>4.28</v>
-      </c>
-      <c r="F16" s="7">
-        <f>E16*A17</f>
-        <v>4.28</v>
-      </c>
-      <c r="G16" s="7">
+        <v>97</v>
+      </c>
+      <c r="E16" s="9">
+        <v>4.96</v>
+      </c>
+      <c r="F16" s="11">
+        <f t="shared" si="1"/>
+        <v>4.96</v>
+      </c>
+      <c r="G16" s="11">
         <f>F16*3</f>
-        <v>12.84</v>
+        <v>14.879999999999999</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>18</v>
@@ -1528,122 +1521,111 @@
       <c r="I16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="K16">
+        <f>3*A16</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="G17" s="11">
+        <f>3*F17</f>
+        <v>13.5</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I17" t="s">
+        <v>94</v>
+      </c>
+      <c r="J17"/>
+      <c r="K17">
         <f>3*A17</f>
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" t="s">
-        <v>114</v>
-      </c>
-      <c r="E17" s="7">
-        <v>4.5</v>
-      </c>
-      <c r="F17" s="7">
-        <f>E17*A18</f>
-        <v>9</v>
-      </c>
-      <c r="G17" s="7">
-        <f>3*F17</f>
-        <v>27</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I17" t="s">
-        <v>97</v>
-      </c>
-      <c r="J17" t="s">
-        <v>38</v>
-      </c>
-      <c r="K17">
-        <f>3*A18</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" ht="15.75">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
-      </c>
-      <c r="E18" s="10">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="F18" s="7">
-        <f>E18*A19</f>
-        <v>0.23400000000000001</v>
-      </c>
-      <c r="G18" s="7">
-        <v>1.17</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>56</v>
+        <v>119</v>
+      </c>
+      <c r="E18" s="8">
+        <v>9.3600000000000003E-2</v>
+      </c>
+      <c r="F18" s="11">
+        <f t="shared" si="1"/>
+        <v>0.18720000000000001</v>
+      </c>
+      <c r="G18" s="8">
+        <v>2.34</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>53</v>
+      </c>
+      <c r="K18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75">
       <c r="A19">
         <v>2</v>
       </c>
       <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E19" s="8">
+        <v>9.3600000000000003E-2</v>
+      </c>
+      <c r="F19" s="11">
+        <f t="shared" si="1"/>
+        <v>0.18720000000000001</v>
+      </c>
+      <c r="G19" s="8">
+        <v>2.34</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" t="s">
-        <v>123</v>
-      </c>
-      <c r="E19" s="7">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="F19" s="7">
-        <f>E19*A20</f>
-        <v>0.23400000000000001</v>
-      </c>
-      <c r="G19" s="7">
-        <v>1.17</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>42</v>
+      <c r="K19" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75">
@@ -1657,29 +1639,26 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="F20" s="11">
+        <f t="shared" si="1"/>
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="G20" s="11">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="E20" s="13">
-        <v>0.41399999999999998</v>
-      </c>
-      <c r="F20" s="7">
-        <f>E20*A21</f>
-        <v>0.41399999999999998</v>
-      </c>
-      <c r="G20" s="7">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1695,14 +1674,14 @@
       <c r="D21" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="11">
         <v>1.94</v>
       </c>
-      <c r="F21" s="7">
-        <f>E21*A22</f>
+      <c r="F21" s="11">
+        <f t="shared" si="1"/>
         <v>1.94</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="11">
         <f>F21*3</f>
         <v>5.82</v>
       </c>
@@ -1712,11 +1691,8 @@
       <c r="I21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="K21">
-        <f>3*A22</f>
+        <f>3*A21</f>
         <v>3</v>
       </c>
     </row>
@@ -1725,35 +1701,32 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D22" t="s">
-        <v>116</v>
-      </c>
-      <c r="E22" s="12">
+        <v>113</v>
+      </c>
+      <c r="E22" s="8">
         <v>1.0229999999999999</v>
       </c>
-      <c r="F22" s="7">
-        <f>E22*A23</f>
-        <v>3.069</v>
-      </c>
-      <c r="G22" s="12">
+      <c r="F22" s="11">
+        <f t="shared" si="1"/>
+        <v>1.0229999999999999</v>
+      </c>
+      <c r="G22" s="8">
         <v>10.23</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>38</v>
+        <v>127</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1762,28 +1735,28 @@
       </c>
       <c r="B23"/>
       <c r="C23" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D23" t="s">
-        <v>98</v>
-      </c>
-      <c r="E23" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>47</v>
+      <c r="G23" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" ht="15.75">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1796,16 +1769,15 @@
       <c r="D24" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="7">
-        <v>0.66</v>
-      </c>
-      <c r="F24" s="7">
-        <f t="shared" ref="F24:F27" si="0">E24*A24</f>
-        <v>0.66</v>
-      </c>
-      <c r="G24" s="7">
-        <f>F24*3</f>
-        <v>1.98</v>
+      <c r="E24" s="10">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="F24" s="11">
+        <f t="shared" ref="F24:F27" si="2">E24*A24</f>
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="G24" s="10">
+        <v>5.42</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>27</v>
@@ -1813,12 +1785,8 @@
       <c r="I24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J24" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K24">
-        <f>3*A24</f>
-        <v>3</v>
+      <c r="K24" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1826,35 +1794,32 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="11">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="F25" s="11">
+        <f t="shared" si="2"/>
+        <v>7.9000000000000015E-2</v>
+      </c>
+      <c r="G25" s="11">
+        <v>1.58</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D25" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="7">
-        <v>1.5800000000000002E-2</v>
-      </c>
-      <c r="F25" s="7">
-        <f t="shared" si="0"/>
-        <v>7.9000000000000015E-2</v>
-      </c>
-      <c r="G25" s="7">
-        <v>1.58</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="K25" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1862,35 +1827,32 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="11">
         <v>1.5800000000000002E-2</v>
       </c>
-      <c r="F26" s="7">
-        <f t="shared" si="0"/>
+      <c r="F26" s="11">
+        <f t="shared" si="2"/>
         <v>1.5800000000000002E-2</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="11">
         <v>1.58</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>62</v>
+      <c r="H26" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="I26" t="s">
-        <v>61</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1901,32 +1863,29 @@
         <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>109</v>
-      </c>
-      <c r="E27" s="7">
+        <v>106</v>
+      </c>
+      <c r="E27" s="11">
         <v>1.5800000000000002E-2</v>
       </c>
-      <c r="F27" s="7">
-        <f t="shared" si="0"/>
+      <c r="F27" s="11">
+        <f t="shared" si="2"/>
         <v>4.7400000000000005E-2</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="11">
         <v>1.58</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>60</v>
+      <c r="H27" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="I27" t="s">
-        <v>90</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1934,25 +1893,25 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D28" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="7" t="s">
-        <v>47</v>
+      <c r="G28" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>32</v>
@@ -1963,33 +1922,30 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C29" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29" s="7">
+        <v>84</v>
+      </c>
+      <c r="E29" s="11">
         <v>2.58</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="11">
         <f>E29*A29</f>
         <v>2.58</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="11">
         <f>F29*3</f>
         <v>7.74</v>
       </c>
       <c r="H29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I29" t="s">
         <v>85</v>
-      </c>
-      <c r="I29" t="s">
-        <v>87</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="K29">
         <f>3*A29</f>
@@ -2007,26 +1963,26 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>136</v>
-      </c>
-      <c r="E31" s="12">
+        <v>132</v>
+      </c>
+      <c r="E31" s="8">
         <v>0.79700000000000004</v>
       </c>
-      <c r="F31" s="7">
-        <f>E31*A31</f>
+      <c r="F31" s="11">
+        <f t="shared" ref="F31:F35" si="3">E31*A31</f>
         <v>0.79700000000000004</v>
       </c>
-      <c r="G31" s="12">
+      <c r="G31" s="8">
         <v>7.97</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I31" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75">
@@ -2034,117 +1990,224 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>139</v>
-      </c>
-      <c r="E32" s="12">
+        <v>135</v>
+      </c>
+      <c r="E32" s="8">
         <v>1.1299999999999999</v>
       </c>
-      <c r="F32" s="7">
-        <f>E32*A32</f>
+      <c r="F32" s="11">
+        <f t="shared" si="3"/>
         <v>1.1299999999999999</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="11">
         <f>F32*3</f>
         <v>3.3899999999999997</v>
       </c>
       <c r="H32" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I32" t="s">
         <v>134</v>
-      </c>
-      <c r="I32" t="s">
-        <v>138</v>
       </c>
       <c r="K32">
         <f>3*A32</f>
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+    <row r="33" spans="1:11" ht="15.75">
+      <c r="A33" s="3">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E33" s="8">
+        <v>1.8320000000000001</v>
+      </c>
+      <c r="F33" s="11">
+        <f t="shared" si="3"/>
+        <v>1.8320000000000001</v>
+      </c>
+      <c r="G33" s="8">
+        <v>9.16</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I33" t="s">
+        <v>148</v>
+      </c>
+      <c r="K33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15.75">
       <c r="A34" s="3">
         <v>1</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="7">
+      <c r="D34" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" s="8">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="F34" s="11">
+        <f t="shared" si="3"/>
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="G34" s="8">
+        <v>3.28</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75">
+      <c r="A35" s="3">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" s="8">
+        <v>5.83</v>
+      </c>
+      <c r="F35" s="11">
+        <f t="shared" si="3"/>
+        <v>5.83</v>
+      </c>
+      <c r="G35" s="11">
+        <f>F35*3</f>
+        <v>17.490000000000002</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="K35">
+        <f>3*A35</f>
         <v>3</v>
-      </c>
-      <c r="F34" s="7">
-        <f>E34*A34</f>
-        <v>3</v>
-      </c>
-      <c r="G34" s="7">
-        <f>F34*3</f>
-        <v>9</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="K34">
-        <f>3*A34</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="D35" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
-      <c r="F36" s="7">
-        <f>SUM(F2:F33)</f>
-        <v>41.62360000000001</v>
-      </c>
-      <c r="G36" s="7">
-        <f>SUM(G2:G33)</f>
-        <v>153.02200000000005</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>125</v>
+      <c r="D36" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="G37" s="11">
-        <f>F36*3-G36</f>
-        <v>-28.151200000000017</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="B40" s="1"/>
+      <c r="D37" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="3">
+        <v>1</v>
+      </c>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" s="14">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="F38" s="11">
+        <f>E38*A38</f>
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="G38" s="14">
+        <v>1.58</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I38" t="s">
+        <v>142</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="3">
+        <v>1</v>
+      </c>
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E39" s="14">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="F39" s="11">
+        <f>E39*A39</f>
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="G39" s="14">
+        <v>1.58</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I39" t="s">
+        <v>144</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="F41" s="11">
+        <f>SUM(F2:F39)</f>
+        <v>42.970300000000002</v>
+      </c>
+      <c r="G41" s="11">
+        <f>SUM(G2:G39)</f>
+        <v>181.03000000000006</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="G42" s="11">
+        <f>F41*3-G41</f>
+        <v>-52.11910000000006</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I42"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="I43"/>
     </row>
   </sheetData>
   <sortState ref="A2:K21">
     <sortCondition ref="C1"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E37:G37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H16" r:id="rId1"/>
@@ -2153,25 +2216,36 @@
     <hyperlink ref="H5" r:id="rId4"/>
     <hyperlink ref="H2" r:id="rId5"/>
     <hyperlink ref="H21" r:id="rId6"/>
-    <hyperlink ref="H20" r:id="rId7"/>
-    <hyperlink ref="H6" r:id="rId8"/>
-    <hyperlink ref="H14" r:id="rId9"/>
-    <hyperlink ref="H4" r:id="rId10"/>
-    <hyperlink ref="H29" r:id="rId11"/>
-    <hyperlink ref="H3" r:id="rId12"/>
-    <hyperlink ref="H7" r:id="rId13"/>
-    <hyperlink ref="H11" r:id="rId14"/>
-    <hyperlink ref="H8" r:id="rId15"/>
-    <hyperlink ref="H17" r:id="rId16"/>
-    <hyperlink ref="H22" r:id="rId17"/>
-    <hyperlink ref="H10" r:id="rId18"/>
-    <hyperlink ref="H32" r:id="rId19"/>
-    <hyperlink ref="H31" r:id="rId20"/>
-    <hyperlink ref="H34" r:id="rId21"/>
-    <hyperlink ref="H35" r:id="rId22"/>
+    <hyperlink ref="H6" r:id="rId7"/>
+    <hyperlink ref="H14" r:id="rId8"/>
+    <hyperlink ref="H4" r:id="rId9"/>
+    <hyperlink ref="H29" r:id="rId10"/>
+    <hyperlink ref="H3" r:id="rId11"/>
+    <hyperlink ref="H7" r:id="rId12"/>
+    <hyperlink ref="H11" r:id="rId13"/>
+    <hyperlink ref="H8" r:id="rId14"/>
+    <hyperlink ref="H22" r:id="rId15"/>
+    <hyperlink ref="H10" r:id="rId16"/>
+    <hyperlink ref="H31" r:id="rId17"/>
+    <hyperlink ref="H37" r:id="rId18"/>
+    <hyperlink ref="H25" r:id="rId19"/>
+    <hyperlink ref="H12" r:id="rId20"/>
+    <hyperlink ref="H9" r:id="rId21"/>
+    <hyperlink ref="H19" r:id="rId22"/>
+    <hyperlink ref="H26" r:id="rId23"/>
+    <hyperlink ref="H27" r:id="rId24"/>
+    <hyperlink ref="H38" r:id="rId25"/>
+    <hyperlink ref="H39" r:id="rId26"/>
+    <hyperlink ref="H18" r:id="rId27"/>
+    <hyperlink ref="H32" r:id="rId28"/>
+    <hyperlink ref="H33" r:id="rId29"/>
+    <hyperlink ref="H34" r:id="rId30" display="http://search.digikey.com/us/en/products/3SB 15-R/507-1537-ND/1009761"/>
+    <hyperlink ref="H35" r:id="rId31"/>
+    <hyperlink ref="H17" r:id="rId32"/>
+    <hyperlink ref="H20" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
 
@@ -2226,13 +2300,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2240,13 +2314,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2254,10 +2328,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -2274,7 +2348,7 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2285,10 +2359,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
         <v>77</v>
-      </c>
-      <c r="D7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2296,13 +2370,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2313,7 +2387,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -2324,13 +2398,13 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2338,13 +2412,13 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2352,13 +2426,13 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2366,10 +2440,10 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2377,13 +2451,13 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2391,13 +2465,13 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2405,13 +2479,13 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2419,13 +2493,13 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2433,13 +2507,13 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2447,13 +2521,13 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2467,7 +2541,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2489,13 +2563,13 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D22" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2503,10 +2577,10 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2528,13 +2602,13 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2542,10 +2616,10 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -2559,10 +2633,10 @@
         <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2570,13 +2644,13 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D28" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2584,13 +2658,13 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C29" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2622,16 +2696,16 @@
         <v>1.9</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
         <v>43</v>
-      </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>